<commit_message>
Added team info in the excel sheet
</commit_message>
<xml_diff>
--- a/RequirementsTemplateM1.xlsx
+++ b/RequirementsTemplateM1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MM\Desktop\test\ashez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samalouty\source\repos\SEproject\SEproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11856" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="Non-Functional Requirements She" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Requirements Sheet'!$A$1:$H$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Requirements Sheet'!$D$1:$D$120</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Team Name</t>
   </si>
@@ -65,24 +65,6 @@
     <t>So that</t>
   </si>
   <si>
-    <t>Schedule</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Create schedules for courses</t>
-  </si>
-  <si>
-    <t>Students &amp; staff can access their schedules</t>
-  </si>
-  <si>
-    <t>View my schedule</t>
-  </si>
-  <si>
-    <t>I can attend my sessions on time</t>
-  </si>
-  <si>
     <t>Measurment</t>
   </si>
   <si>
@@ -95,20 +77,86 @@
     <t>Mobile App or Website or Both</t>
   </si>
   <si>
-    <t>This is just an example. The schedule module is repsonsible for handling the personalized schedule of the course for each stakeholder.</t>
-  </si>
-  <si>
     <t>Students</t>
   </si>
   <si>
-    <t>Hazem</t>
+    <t>Habiba Hesham Elsonbaty</t>
+  </si>
+  <si>
+    <t>55-0966</t>
+  </si>
+  <si>
+    <t>T-21</t>
+  </si>
+  <si>
+    <t>Abdelrahman Hesham Elsamalouty</t>
+  </si>
+  <si>
+    <t>55-0842</t>
+  </si>
+  <si>
+    <t>Abdelrahman Ahmed Elaby</t>
+  </si>
+  <si>
+    <t>55-0990</t>
+  </si>
+  <si>
+    <t>Ehab Medhat Ehab</t>
+  </si>
+  <si>
+    <t>55-4571</t>
+  </si>
+  <si>
+    <t>Hazem Mohamed Mansour</t>
+  </si>
+  <si>
+    <t>55-1036</t>
+  </si>
+  <si>
+    <t>Zeina Mohamed Fadel</t>
+  </si>
+  <si>
+    <t>55-1095</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>client/banker/admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be able to login  </t>
+  </si>
+  <si>
+    <t>I have access to the application</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>zeina.abdeen@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>ehab.abdelkader@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>abdelrahman.elaby@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>Hazem.alfedawy@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>abdelrahman.shawky@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>habiba.elsonbaty@student.guc.edu.eg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -198,6 +246,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -219,7 +280,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -242,11 +303,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,12 +363,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -301,8 +383,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -521,49 +626,49 @@
   </sheetPr>
   <dimension ref="A1:D998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
     <col min="3" max="3" width="46.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>24</v>
+      <c r="A5" s="19" t="s">
+        <v>17</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -580,40 +685,88 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1602,13 +1755,19 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sortState ref="A7:D12">
+    <sortCondition ref="A7"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D4"/>
     <mergeCell ref="A5:D5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1619,15 +1778,15 @@
   </sheetPr>
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" customWidth="1"/>
     <col min="5" max="6" width="35.5546875" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="54.88671875" customWidth="1"/>
@@ -1666,76 +1825,55 @@
       <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>22</v>
+      <c r="G2" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>31</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
+      <c r="B3" s="26">
+        <v>1</v>
       </c>
       <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
+      <c r="D3" s="27" t="s">
+        <v>32</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>16</v>
+      <c r="E3" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12" t="s">
-        <v>23</v>
+      <c r="F3" s="14" t="s">
+        <v>34</v>
       </c>
+      <c r="G3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10">
-        <v>3</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="10"/>
-    </row>
+      <c r="A4" s="20"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="10"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -2879,11 +3017,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G120">
+    <dataValidation type="list" allowBlank="1" sqref="D1:D4 D6:D120">
+      <formula1>"client,banker,admin,client/banker,banker/admin,client/admin,client/banker/admin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G6:G120 G3:G4">
       <formula1>"Mobile App,Online Banking Website,Both"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D1:D120">
-      <formula1>"client,banker,admin,client/banker,banker/admin,client/admin,client/banker/admin"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2899,7 +3037,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2912,20 +3050,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>20</v>
+      <c r="E1" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2950,9 +3088,9 @@
     </row>
     <row r="2" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="10"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>

</xml_diff>

<commit_message>
added the first requirements
</commit_message>
<xml_diff>
--- a/RequirementsTemplateM1.xlsx
+++ b/RequirementsTemplateM1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11856" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Team Name</t>
   </si>
@@ -119,18 +119,6 @@
     <t>55-1095</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>client/banker/admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Be able to login  </t>
-  </si>
-  <si>
-    <t>I have access to the application</t>
-  </si>
-  <si>
     <t>Both</t>
   </si>
   <si>
@@ -151,12 +139,84 @@
   <si>
     <t>habiba.elsonbaty@student.guc.edu.eg</t>
   </si>
+  <si>
+    <t>donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donor/receiver/delivery person/admin </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to sign up </t>
+  </si>
+  <si>
+    <t>so that I can create an account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> so that I have access to the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to have a location map </t>
+  </si>
+  <si>
+    <t>so that I know the nearest blood drive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view all available hospitals </t>
+  </si>
+  <si>
+    <t>so that I check the blood demand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view all blood demand requests </t>
+  </si>
+  <si>
+    <t>so that I check the suitable blood type.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view a list of blood requests sorted with urgency </t>
+  </si>
+  <si>
+    <t>so that I can donate to the highest priority first.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view a list of all requested medication names </t>
+  </si>
+  <si>
+    <t>so that I check if the medicine I want to donate is needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view dr appointment requests </t>
+  </si>
+  <si>
+    <t>so that I can choose the suitable appointment according to my profession.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to schedule dr appointments with patients </t>
+  </si>
+  <si>
+    <t>so that I can choose the suitable timing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to cancel previously scheduled appointments </t>
+  </si>
+  <si>
+    <t>so that another donor could benefit the patient if I have an emergency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I should be able to view the age of the patient </t>
+  </si>
+  <si>
+    <t>so that I use the suitable equipment and treatment in the appointment.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,6 +319,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -334,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +439,20 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,28 +464,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,7 +712,7 @@
   </sheetPr>
   <dimension ref="A1:D998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -637,38 +723,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -692,7 +778,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
@@ -706,7 +792,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -720,7 +806,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>20</v>
@@ -733,8 +819,8 @@
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>41</v>
+      <c r="C10" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>20</v>
@@ -748,7 +834,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>20</v>
@@ -762,7 +848,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -1778,18 +1864,20 @@
   </sheetPr>
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" customWidth="1"/>
-    <col min="5" max="6" width="35.5546875" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="54.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1831,118 +1919,222 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="26">
-        <v>1</v>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="33">
+        <v>2</v>
       </c>
-      <c r="C3" s="10">
-        <v>1</v>
+      <c r="D4" s="15" t="s">
+        <v>39</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>32</v>
+      <c r="E4" s="26" t="s">
+        <v>42</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>33</v>
+      <c r="F4" s="28" t="s">
+        <v>43</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>34</v>
+      <c r="G4" s="11" t="s">
+        <v>31</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>35</v>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="34">
+        <v>3</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-    </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="23"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="32">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="C7" s="33">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="C8" s="34">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="C9" s="32">
+        <v>7</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
+      <c r="C10" s="33">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="C11" s="34">
+        <v>9</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="C12" s="32">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
+      <c r="C13" s="33">
+        <v>11</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3017,11 +3209,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="D1:D4 D6:D120">
-      <formula1>"client,banker,admin,client/banker,banker/admin,client/admin,client/banker/admin"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G120">
+      <formula1>"Mobile App,Online Banking Website,Both"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G6:G120 G3:G4">
-      <formula1>"Mobile App,Online Banking Website,Both"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="D1:D1048576">
+      <formula1>"client,banker,admin,client/banker,banker/admin,client/admin,client/banker/admin, donor, receiver, delivery person, Donor/receiver/delivery person/admin "</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated some Health module requirements
</commit_message>
<xml_diff>
--- a/RequirementsTemplateM1.xlsx
+++ b/RequirementsTemplateM1.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Non-Functional Requirements She" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Requirements Sheet'!$D$1:$D$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Requirements Sheet'!$D$1:$D$123</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Team Name</t>
   </si>
@@ -155,16 +155,10 @@
     <t>I know the nearest blood drive.</t>
   </si>
   <si>
-    <t>I check the blood demand.</t>
-  </si>
-  <si>
     <t>I check the suitable blood type.</t>
   </si>
   <si>
     <t>I can donate to the highest priority first.</t>
-  </si>
-  <si>
-    <t>I check if the medicine I want to donate is needed.</t>
   </si>
   <si>
     <t>I can choose the suitable appointment according to my profession.</t>
@@ -185,19 +179,10 @@
     <t>Be able to login.</t>
   </si>
   <si>
-    <t>Be able to have a location map.</t>
-  </si>
-  <si>
     <t>Be able to view all available hospitals.</t>
   </si>
   <si>
-    <t>Be able to view all blood demand requests.</t>
-  </si>
-  <si>
     <t>Be able to view a list of blood requests sorted with urgency.</t>
-  </si>
-  <si>
-    <t>Be able to view a list of all requested medication names.</t>
   </si>
   <si>
     <t>Be able to view dr appointment requests.</t>
@@ -210,6 +195,42 @@
   </si>
   <si>
     <t>Be able to view the age of the patient.</t>
+  </si>
+  <si>
+    <t>Health sector donations</t>
+  </si>
+  <si>
+    <t>Be able to view all blood demand requests in a certain hospital.</t>
+  </si>
+  <si>
+    <t>Be able to have a blood drive location map.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can check information about a certain hospital. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be able to view how much of a certain medicine is needed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can know how much to buy or donate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can check if I have the medication/supplies needed for donation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be able to filter the type of medication/supplies. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can find the needed medicine/supply by name. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be able to search through all needed medicine/supply by exact name. </t>
+  </si>
+  <si>
+    <t>Be able to view a list of all requested medication/supply names.</t>
+  </si>
+  <si>
+    <t>I check if the medicine/supply I want to donate is needed.</t>
   </si>
 </sst>
 </file>
@@ -347,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -396,12 +417,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,9 +498,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -465,6 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,6 +518,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1847,15 +1903,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
@@ -1904,20 +1960,20 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>1</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="11" t="s">
@@ -1926,18 +1982,18 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="23">
+      <c r="A4" s="5"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="22">
         <v>2</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="21" t="s">
+      <c r="E4" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="11" t="s">
@@ -1946,16 +2002,20 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="24">
+      <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="23">
         <v>3</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="E5" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -1963,19 +2023,21 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="22">
+      <c r="A6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="21">
         <v>4</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>43</v>
+      <c r="E6" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>31</v>
@@ -1983,19 +2045,21 @@
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="23">
+      <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="22">
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>44</v>
+      <c r="E7" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>31</v>
@@ -2003,19 +2067,21 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="24">
+      <c r="A8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="23">
         <v>6</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>45</v>
+      <c r="E8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>31</v>
@@ -2023,79 +2089,81 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="22">
+      <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="21">
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>46</v>
+      <c r="E9" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="23">
+    <row r="10" spans="1:8" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="21">
         <v>8</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>47</v>
+      <c r="E10" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>63</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>31</v>
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="24">
+    <row r="11" spans="1:8" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="22">
         <v>9</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>48</v>
+      <c r="E11" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>65</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="22">
+    <row r="12" spans="1:8" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="23">
         <v>10</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>49</v>
+      <c r="E12" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>31</v>
@@ -2103,19 +2171,21 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="23">
+      <c r="A13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="21">
         <v>11</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>50</v>
+      <c r="E13" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>31</v>
@@ -2123,42 +2193,78 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
+      <c r="A14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="22">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="23">
+        <v>13</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
+      <c r="A16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="21">
+        <v>14</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="11"/>
       <c r="H17" s="10"/>
     </row>
@@ -3192,9 +3298,39 @@
       <c r="G120" s="11"/>
       <c r="H120" s="10"/>
     </row>
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="10"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="10"/>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="10"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="11"/>
+      <c r="H122" s="10"/>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="11"/>
+      <c r="H123" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G120">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G123">
       <formula1>"Mobile App,Online Banking Website,Both"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D1:D1048576">

</xml_diff>

<commit_message>
Update 110 Functional requirements
finished school supplies, ("el fo2eeha "changed to actual cell references), added some requirements for the orphanage donations
</commit_message>
<xml_diff>
--- a/RequirementsTemplateM1.xlsx
+++ b/RequirementsTemplateM1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Habiba\Documents\GitHub\ashez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samalouty\source\repos\SEproject\SEproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20740" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Requirements Sheet'!$D$1:$D$142</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="283">
   <si>
     <t>Name</t>
   </si>
@@ -219,9 +219,6 @@
     <t xml:space="preserve">I can choose what I am experienced at to benefit people's welfare </t>
   </si>
   <si>
-    <t>communicate with the tutoring students</t>
-  </si>
-  <si>
     <t>I can assign to them tasks and homework</t>
   </si>
   <si>
@@ -531,9 +528,6 @@
     <t>offer free transportation means for pro bono appointments and tutoring</t>
   </si>
   <si>
-    <t>it can be easier to go.</t>
-  </si>
-  <si>
     <t>I can quickly update the receivers and donors of my current status</t>
   </si>
   <si>
@@ -636,18 +630,12 @@
     <t>Have the option to donate to a school</t>
   </si>
   <si>
-    <t>el fo2eeha</t>
-  </si>
-  <si>
     <t>I can notify interested receivers that new books are offered if they need it</t>
   </si>
   <si>
     <t>I can check the requested school supply by type/brand/quality</t>
   </si>
   <si>
-    <t>I can to donate to schools insteadmof an individual or organization</t>
-  </si>
-  <si>
     <t>I can pick the school to donate to</t>
   </si>
   <si>
@@ -822,9 +810,6 @@
     <t xml:space="preserve">So that the orphanage categorizes these toys based on age.               </t>
   </si>
   <si>
-    <t>So that the orphanage categorizes these supplies based on the type</t>
-  </si>
-  <si>
     <t>Be able to specify the type of supplies(pencil/pen/ruler/book)</t>
   </si>
   <si>
@@ -835,12 +820,66 @@
   </si>
   <si>
     <t>I can choose from toys,school supplies,luxury foods .. Etc.</t>
+  </si>
+  <si>
+    <t>Be able to specify the type of luxury food</t>
+  </si>
+  <si>
+    <t>Be able to insert ingredients of the luxury food</t>
+  </si>
+  <si>
+    <t>calories and nutritional value can be calculated to not feed orphans nutritionally unsuitable food (lactose intolerant people don't get food that contains lactose)</t>
+  </si>
+  <si>
+    <t>the orphanage categorizes these supplies based on the type of supply</t>
+  </si>
+  <si>
+    <t>the orphanage categorizes these supplies based on the type of food</t>
+  </si>
+  <si>
+    <t>donation receivers who are unable to pay for transportation can get the pro bono appointments</t>
+  </si>
+  <si>
+    <t>Specify the course in which he needs a tutoring session</t>
+  </si>
+  <si>
+    <t>I can find the proper tutor for my tutoring needs</t>
+  </si>
+  <si>
+    <t>Specify the grade of the book needed (year 9, year 10,..)</t>
+  </si>
+  <si>
+    <t>Specify the quantity and the types of supplies needed (via 2 dropdown lists for example)</t>
+  </si>
+  <si>
+    <t>I can get the relevant books for my correct year</t>
+  </si>
+  <si>
+    <t>I can get the actual supplies I need and not redundant supplies</t>
+  </si>
+  <si>
+    <t>communicate with the tutoring students via messages</t>
+  </si>
+  <si>
+    <t>I can to donate to schools instead of an individual or organization</t>
+  </si>
+  <si>
+    <t>add the locations of schools that accept donations</t>
+  </si>
+  <si>
+    <t>the donor can select which school to donate to</t>
+  </si>
+  <si>
+    <t>send notifications for needed items which are running low on stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the donors know which items are more needed </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1083,7 +1122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1203,6 +1242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1429,15 +1471,15 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="46.6328125" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1461,7 +1503,7 @@
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>16</v>
       </c>
@@ -1469,7 +1511,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1497,7 +1539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1511,7 +1553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1525,7 +1567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1539,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -2577,20 +2619,20 @@
   </sheetPr>
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.453125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.90625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.453125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.44140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="102.44140625" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2633,17 +2675,17 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="18">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>39</v>
@@ -2655,7 +2697,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="19">
@@ -2665,7 +2707,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>40</v>
@@ -2677,7 +2719,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="18">
@@ -2687,10 +2729,10 @@
         <v>37</v>
       </c>
       <c r="E5" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>30</v>
@@ -2699,7 +2741,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="19">
@@ -2709,10 +2751,10 @@
         <v>37</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>30</v>
@@ -2721,7 +2763,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="18">
@@ -2731,10 +2773,10 @@
         <v>37</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>133</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>30</v>
@@ -2743,7 +2785,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="19">
@@ -2753,10 +2795,10 @@
         <v>37</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>30</v>
@@ -2765,7 +2807,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="18">
@@ -2775,10 +2817,10 @@
         <v>37</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>30</v>
@@ -2787,7 +2829,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="19">
@@ -2797,10 +2839,10 @@
         <v>37</v>
       </c>
       <c r="E10" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>158</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>30</v>
@@ -2809,7 +2851,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="18">
@@ -2819,10 +2861,10 @@
         <v>46</v>
       </c>
       <c r="E11" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>142</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>30</v>
@@ -2831,7 +2873,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="19">
@@ -2841,10 +2883,10 @@
         <v>37</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>160</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>30</v>
@@ -2853,7 +2895,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="18">
@@ -2863,10 +2905,10 @@
         <v>37</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>30</v>
@@ -2875,7 +2917,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="19">
@@ -2885,10 +2927,10 @@
         <v>53</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>30</v>
@@ -2897,7 +2939,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="18">
@@ -2907,24 +2949,24 @@
         <v>37</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="39" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="19">
         <v>14</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -2943,7 +2985,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>41</v>
@@ -2987,7 +3029,7 @@
         <v>37</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>43</v>
@@ -2997,7 +3039,7 @@
       </c>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>45</v>
       </c>
@@ -3009,7 +3051,7 @@
         <v>46</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>49</v>
@@ -3019,7 +3061,7 @@
       </c>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>45</v>
       </c>
@@ -3041,7 +3083,7 @@
       </c>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>45</v>
       </c>
@@ -3053,17 +3095,17 @@
         <v>46</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>30</v>
       </c>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>45</v>
       </c>
@@ -3075,17 +3117,17 @@
         <v>46</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>45</v>
       </c>
@@ -3097,17 +3139,17 @@
         <v>46</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>30</v>
       </c>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>45</v>
       </c>
@@ -3119,10 +3161,10 @@
         <v>46</v>
       </c>
       <c r="E25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>85</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>30</v>
@@ -3141,10 +3183,10 @@
         <v>46</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>30</v>
@@ -3163,7 +3205,7 @@
         <v>46</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>47</v>
@@ -3185,7 +3227,7 @@
         <v>46</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>48</v>
@@ -3217,7 +3259,7 @@
       </c>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>45</v>
       </c>
@@ -3251,7 +3293,7 @@
         <v>53</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>58</v>
@@ -3273,7 +3315,7 @@
         <v>53</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>58</v>
@@ -3298,7 +3340,7 @@
         <v>60</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>30</v>
@@ -3309,8 +3351,9 @@
       <c r="A34" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>203</v>
+      <c r="B34" s="10">
+        <f>C33</f>
+        <v>31</v>
       </c>
       <c r="C34" s="19">
         <v>32</v>
@@ -3319,10 +3362,10 @@
         <v>37</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>30</v>
@@ -3341,10 +3384,10 @@
         <v>37</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>30</v>
@@ -3363,10 +3406,10 @@
         <v>37</v>
       </c>
       <c r="E36" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>30</v>
@@ -3399,8 +3442,9 @@
       <c r="A38" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>203</v>
+      <c r="B38" s="10">
+        <f>C37</f>
+        <v>35</v>
       </c>
       <c r="C38" s="19">
         <v>36</v>
@@ -3409,10 +3453,10 @@
         <v>37</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="10"/>
@@ -3429,10 +3473,10 @@
         <v>37</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G39" s="11"/>
       <c r="H39" s="10"/>
@@ -3449,10 +3493,10 @@
         <v>37</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="10"/>
@@ -3469,10 +3513,10 @@
         <v>37</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="10"/>
@@ -3481,8 +3525,9 @@
       <c r="A42" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>203</v>
+      <c r="B42" s="10">
+        <f>C41</f>
+        <v>39</v>
       </c>
       <c r="C42" s="19">
         <v>40</v>
@@ -3491,10 +3536,10 @@
         <v>37</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="10"/>
@@ -3511,10 +3556,10 @@
         <v>37</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="10"/>
@@ -3531,10 +3576,10 @@
         <v>37</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G44" s="11" t="s">
         <v>30</v>
@@ -3553,7 +3598,7 @@
         <v>37</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>63</v>
@@ -3575,10 +3620,10 @@
         <v>37</v>
       </c>
       <c r="E46" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="F46" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>30</v>
@@ -3597,10 +3642,10 @@
         <v>37</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>30</v>
@@ -3619,10 +3664,10 @@
         <v>46</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>30</v>
@@ -3641,10 +3686,10 @@
         <v>46</v>
       </c>
       <c r="E49" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F49" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>77</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>30</v>
@@ -3663,10 +3708,10 @@
         <v>46</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F50" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G50" s="11" t="s">
         <v>30</v>
@@ -3685,10 +3730,10 @@
         <v>46</v>
       </c>
       <c r="E51" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>91</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>30</v>
@@ -3707,10 +3752,10 @@
         <v>46</v>
       </c>
       <c r="E52" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="F52" s="20" t="s">
         <v>211</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>215</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="10"/>
@@ -3727,10 +3772,10 @@
         <v>46</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>30</v>
@@ -3749,10 +3794,10 @@
         <v>46</v>
       </c>
       <c r="E54" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="G54" s="11" t="s">
         <v>30</v>
@@ -3771,10 +3816,10 @@
         <v>37</v>
       </c>
       <c r="E55" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G55" s="28" t="s">
         <v>30</v>
@@ -3793,10 +3838,10 @@
         <v>53</v>
       </c>
       <c r="E56" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>30</v>
@@ -3807,13 +3852,22 @@
       <c r="A57" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="10"/>
+      <c r="B57" s="10">
+        <f>C51</f>
+        <v>49</v>
+      </c>
       <c r="C57" s="18">
         <v>55</v>
       </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
+      <c r="D57" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>272</v>
+      </c>
       <c r="G57" s="28"/>
       <c r="H57" s="10"/>
     </row>
@@ -3821,13 +3875,22 @@
       <c r="A58" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="10"/>
+      <c r="B58" s="10">
+        <f xml:space="preserve"> C54</f>
+        <v>52</v>
+      </c>
       <c r="C58" s="19">
         <v>56</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="D58" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>275</v>
+      </c>
       <c r="G58" s="28"/>
       <c r="H58" s="10"/>
     </row>
@@ -3835,13 +3898,22 @@
       <c r="A59" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="10"/>
+      <c r="B59" s="10">
+        <f xml:space="preserve"> C53</f>
+        <v>51</v>
+      </c>
       <c r="C59" s="18">
         <v>57</v>
       </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
+      <c r="D59" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>276</v>
+      </c>
       <c r="G59" s="28"/>
       <c r="H59" s="10"/>
     </row>
@@ -3853,9 +3925,15 @@
       <c r="C60" s="19">
         <v>58</v>
       </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="D60" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>280</v>
+      </c>
       <c r="G60" s="28"/>
       <c r="H60" s="10"/>
     </row>
@@ -3867,15 +3945,21 @@
       <c r="C61" s="18">
         <v>59</v>
       </c>
-      <c r="D61" s="9"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="D61" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>282</v>
+      </c>
       <c r="G61" s="28"/>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="19">
@@ -3885,10 +3969,10 @@
         <v>37</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>168</v>
+        <v>270</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>30</v>
@@ -3897,7 +3981,7 @@
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="18">
@@ -3907,10 +3991,10 @@
         <v>51</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>30</v>
@@ -3919,20 +4003,20 @@
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="19">
         <v>62</v>
       </c>
       <c r="D64" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E64" s="20" t="s">
+      <c r="F64" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="G64" s="28" t="s">
         <v>30</v>
@@ -3941,7 +4025,7 @@
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="18">
@@ -3951,10 +4035,10 @@
         <v>53</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G65" s="28" t="s">
         <v>30</v>
@@ -3963,20 +4047,20 @@
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="19">
         <v>64</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E66" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="F66" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="G66" s="28" t="s">
         <v>30</v>
@@ -3985,20 +4069,20 @@
     </row>
     <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="18">
         <v>65</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G67" s="28" t="s">
         <v>30</v>
@@ -4007,20 +4091,20 @@
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="19">
         <v>66</v>
       </c>
       <c r="D68" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="F68" s="20" t="s">
         <v>138</v>
-      </c>
-      <c r="E68" s="29" t="s">
-        <v>251</v>
-      </c>
-      <c r="F68" s="20" t="s">
-        <v>139</v>
       </c>
       <c r="G68" s="28" t="s">
         <v>30</v>
@@ -4029,20 +4113,20 @@
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="18">
         <v>67</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>30</v>
@@ -4051,7 +4135,7 @@
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="19">
@@ -4061,10 +4145,10 @@
         <v>51</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G70" s="28" t="s">
         <v>30</v>
@@ -4073,7 +4157,7 @@
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="18">
@@ -4083,10 +4167,10 @@
         <v>51</v>
       </c>
       <c r="E71" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F71" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>105</v>
       </c>
       <c r="G71" s="28" t="s">
         <v>30</v>
@@ -4095,7 +4179,7 @@
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="19">
@@ -4105,10 +4189,10 @@
         <v>51</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G72" s="28" t="s">
         <v>30</v>
@@ -4117,7 +4201,7 @@
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="18">
@@ -4127,10 +4211,10 @@
         <v>51</v>
       </c>
       <c r="E73" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F73" s="20" t="s">
         <v>109</v>
-      </c>
-      <c r="F73" s="20" t="s">
-        <v>110</v>
       </c>
       <c r="G73" s="28" t="s">
         <v>30</v>
@@ -4139,7 +4223,7 @@
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="19">
@@ -4149,10 +4233,10 @@
         <v>46</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G74" s="28" t="s">
         <v>30</v>
@@ -4161,20 +4245,20 @@
     </row>
     <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="18">
         <v>73</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E75" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F75" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>113</v>
       </c>
       <c r="G75" s="28" t="s">
         <v>30</v>
@@ -4183,20 +4267,20 @@
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="19">
         <v>74</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G76" s="28" t="s">
         <v>30</v>
@@ -4205,20 +4289,20 @@
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="18">
         <v>75</v>
       </c>
       <c r="D77" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E77" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E77" s="20" t="s">
+      <c r="F77" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="F77" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="G77" s="28" t="s">
         <v>30</v>
@@ -4227,7 +4311,7 @@
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="19">
@@ -4237,10 +4321,10 @@
         <v>53</v>
       </c>
       <c r="E78" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F78" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="G78" s="28" t="s">
         <v>30</v>
@@ -4249,20 +4333,20 @@
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="18">
         <v>77</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G79" s="28" t="s">
         <v>30</v>
@@ -4271,20 +4355,20 @@
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="19">
         <v>78</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>30</v>
@@ -4293,7 +4377,7 @@
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="18">
@@ -4303,10 +4387,10 @@
         <v>51</v>
       </c>
       <c r="E81" s="20" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>30</v>
@@ -4315,7 +4399,7 @@
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="19">
@@ -4325,10 +4409,10 @@
         <v>51</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>30</v>
@@ -4337,7 +4421,7 @@
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="18">
@@ -4347,10 +4431,10 @@
         <v>51</v>
       </c>
       <c r="E83" s="20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G83" s="11" t="s">
         <v>30</v>
@@ -4359,7 +4443,7 @@
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="19">
@@ -4369,10 +4453,10 @@
         <v>37</v>
       </c>
       <c r="E84" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G84" s="11" t="s">
         <v>30</v>
@@ -4381,7 +4465,7 @@
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="18">
@@ -4391,10 +4475,10 @@
         <v>37</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>30</v>
@@ -4403,7 +4487,7 @@
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="19">
@@ -4413,10 +4497,10 @@
         <v>46</v>
       </c>
       <c r="E86" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="F86" s="20" t="s">
-        <v>129</v>
       </c>
       <c r="G86" s="11" t="s">
         <v>30</v>
@@ -4425,7 +4509,7 @@
     </row>
     <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="18">
@@ -4435,10 +4519,10 @@
         <v>46</v>
       </c>
       <c r="E87" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F87" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="F87" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>30</v>
@@ -4447,7 +4531,7 @@
     </row>
     <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="19">
@@ -4457,10 +4541,10 @@
         <v>37</v>
       </c>
       <c r="E88" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F88" s="20" t="s">
         <v>143</v>
-      </c>
-      <c r="F88" s="20" t="s">
-        <v>144</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>30</v>
@@ -4469,7 +4553,7 @@
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="18">
@@ -4479,10 +4563,10 @@
         <v>37</v>
       </c>
       <c r="E89" s="20" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>30</v>
@@ -4491,7 +4575,7 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="19">
@@ -4501,10 +4585,10 @@
         <v>37</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>30</v>
@@ -4513,7 +4597,7 @@
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="18">
@@ -4523,10 +4607,10 @@
         <v>37</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>30</v>
@@ -4535,7 +4619,7 @@
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="19">
@@ -4545,17 +4629,17 @@
         <v>37</v>
       </c>
       <c r="E92" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="18">
@@ -4565,17 +4649,17 @@
         <v>37</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G93" s="11"/>
       <c r="H93" s="10"/>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="19">
@@ -4585,10 +4669,10 @@
         <v>37</v>
       </c>
       <c r="E94" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>30</v>
@@ -4597,7 +4681,7 @@
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="18">
@@ -4607,10 +4691,10 @@
         <v>46</v>
       </c>
       <c r="E95" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F95" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="F95" s="20" t="s">
-        <v>150</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>30</v>
@@ -4619,7 +4703,7 @@
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="19">
@@ -4629,10 +4713,10 @@
         <v>37</v>
       </c>
       <c r="E96" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F96" s="20" t="s">
         <v>151</v>
-      </c>
-      <c r="F96" s="20" t="s">
-        <v>152</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>30</v>
@@ -4641,7 +4725,7 @@
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="18">
@@ -4651,10 +4735,10 @@
         <v>37</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G97" s="11" t="s">
         <v>30</v>
@@ -4663,7 +4747,7 @@
     </row>
     <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="19">
@@ -4673,10 +4757,10 @@
         <v>37</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F98" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G98" s="11" t="s">
         <v>30</v>
@@ -4685,7 +4769,7 @@
     </row>
     <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="18">
@@ -4695,10 +4779,10 @@
         <v>37</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G99" s="11" t="s">
         <v>30</v>
@@ -4707,7 +4791,7 @@
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B100" s="10"/>
       <c r="C100" s="19">
@@ -4717,10 +4801,10 @@
         <v>46</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G100" s="11" t="s">
         <v>30</v>
@@ -4729,7 +4813,7 @@
     </row>
     <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="18">
@@ -4739,10 +4823,10 @@
         <v>53</v>
       </c>
       <c r="E101" s="20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>30</v>
@@ -4751,7 +4835,7 @@
     </row>
     <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="19">
@@ -4761,10 +4845,10 @@
         <v>37</v>
       </c>
       <c r="E102" s="20" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>30</v>
@@ -4773,7 +4857,7 @@
     </row>
     <row r="103" spans="1:8" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B103" s="10"/>
       <c r="C103" s="18">
@@ -4783,10 +4867,10 @@
         <v>37</v>
       </c>
       <c r="E103" s="20" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>30</v>
@@ -4795,9 +4879,10 @@
     </row>
     <row r="104" spans="1:8" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B104" s="10">
+        <f>C103</f>
         <v>101</v>
       </c>
       <c r="C104" s="19">
@@ -4807,10 +4892,10 @@
         <v>37</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>30</v>
@@ -4819,7 +4904,7 @@
     </row>
     <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="18">
@@ -4829,10 +4914,10 @@
         <v>37</v>
       </c>
       <c r="E105" s="20" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>30</v>
@@ -4841,7 +4926,7 @@
     </row>
     <row r="106" spans="1:8" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B106" s="10"/>
       <c r="C106" s="19">
@@ -4851,10 +4936,10 @@
         <v>37</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>30</v>
@@ -4863,7 +4948,7 @@
     </row>
     <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B107" s="10"/>
       <c r="C107" s="18">
@@ -4873,10 +4958,10 @@
         <v>37</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>30</v>
@@ -4885,7 +4970,7 @@
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="19">
@@ -4895,10 +4980,10 @@
         <v>37</v>
       </c>
       <c r="E108" s="20" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F108" s="20" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>30</v>
@@ -4907,7 +4992,7 @@
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B109" s="10"/>
       <c r="C109" s="18">
@@ -4917,10 +5002,10 @@
         <v>37</v>
       </c>
       <c r="E109" s="20" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F109" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>30</v>
@@ -4929,7 +5014,7 @@
     </row>
     <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B110" s="10"/>
       <c r="C110" s="19">
@@ -4939,10 +5024,10 @@
         <v>37</v>
       </c>
       <c r="E110" s="20" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F110" s="20" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>30</v>
@@ -4951,7 +5036,7 @@
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B111" s="10"/>
       <c r="C111" s="18">
@@ -4961,10 +5046,10 @@
         <v>37</v>
       </c>
       <c r="E111" s="20" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F111" s="20" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>30</v>
@@ -4973,7 +5058,7 @@
     </row>
     <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B112" s="10"/>
       <c r="C112" s="19">
@@ -4982,28 +5067,45 @@
       <c r="D112" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="11"/>
+      <c r="E112" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H112" s="10"/>
     </row>
-    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B113" s="10"/>
+        <v>228</v>
+      </c>
+      <c r="B113" s="10">
+        <f>C112</f>
+        <v>110</v>
+      </c>
       <c r="C113" s="18">
         <v>111</v>
       </c>
-      <c r="D113" s="9"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="11"/>
+      <c r="D113" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="F113" s="48" t="s">
+        <v>267</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H113" s="10"/>
     </row>
     <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B114" s="10"/>
       <c r="C114" s="19">
@@ -5017,7 +5119,7 @@
     </row>
     <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B115" s="10"/>
       <c r="C115" s="18">
@@ -5031,7 +5133,7 @@
     </row>
     <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B116" s="10"/>
       <c r="C116" s="19">
@@ -5045,7 +5147,7 @@
     </row>
     <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B117" s="10"/>
       <c r="C117" s="18">
@@ -5059,7 +5161,7 @@
     </row>
     <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B118" s="10"/>
       <c r="C118" s="19">
@@ -5073,7 +5175,7 @@
     </row>
     <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B119" s="10"/>
       <c r="C119" s="18">
@@ -5087,7 +5189,7 @@
     </row>
     <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B120" s="10"/>
       <c r="C120" s="19">
@@ -5101,7 +5203,7 @@
     </row>
     <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B121" s="10"/>
       <c r="C121" s="18">
@@ -5115,7 +5217,7 @@
     </row>
     <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B122" s="10"/>
       <c r="C122" s="19">
@@ -5129,7 +5231,7 @@
     </row>
     <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B123" s="10"/>
       <c r="C123" s="18">
@@ -5143,7 +5245,7 @@
     </row>
     <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B124" s="10"/>
       <c r="C124" s="19">
@@ -5157,7 +5259,7 @@
     </row>
     <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B125" s="10"/>
       <c r="C125" s="18">
@@ -5597,13 +5699,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="93.453125" customWidth="1"/>
-    <col min="4" max="4" width="118.54296875" customWidth="1"/>
-    <col min="5" max="5" width="51.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="93.44140625" customWidth="1"/>
+    <col min="4" max="4" width="118.5546875" customWidth="1"/>
+    <col min="5" max="5" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5675,10 +5777,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -5708,10 +5810,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5741,10 +5843,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -5774,10 +5876,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -5807,10 +5909,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -5840,10 +5942,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -5873,10 +5975,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -5906,10 +6008,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -5939,10 +6041,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -12404,9 +12506,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.81640625" customWidth="1"/>
+    <col min="1" max="1" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -12426,7 +12528,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -12436,22 +12538,22 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>